<commit_message>
Validated UE 2000–2018 against previous work
</commit_message>
<xml_diff>
--- a/data/analysis/pivot-by-state.xlsx
+++ b/data/analysis/pivot-by-state.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alecramsay/dev/ushouse/data/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6096641-8A28-534D-8A03-E1C4E5E1D993}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B87A66D-3A14-E943-BF66-9EFE5792D224}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11580" yWindow="5400" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{243A2677-B725-5B4A-8946-B944A46BAF00}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="123">
   <si>
     <t>XX</t>
   </si>
@@ -962,35 +962,35 @@
       <c r="B3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>15</v>
+      <c r="C3" s="7">
+        <v>0</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0</v>
+      </c>
+      <c r="F3" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="H3" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="I3" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="J3" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="K3" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="L3" s="7">
+        <v>0.5</v>
       </c>
       <c r="M3" s="7" t="s">
         <v>15</v>
@@ -1208,35 +1208,35 @@
       <c r="B9" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K9" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="L9" s="7" t="s">
-        <v>15</v>
+      <c r="C9" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D9" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="E9" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="F9" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="G9" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="H9" s="7">
+        <v>-0.5</v>
+      </c>
+      <c r="I9" s="7">
+        <v>-0.5</v>
+      </c>
+      <c r="J9" s="7">
+        <v>-0.5</v>
+      </c>
+      <c r="K9" s="7">
+        <v>-0.5</v>
+      </c>
+      <c r="L9" s="7">
+        <v>-0.5</v>
       </c>
       <c r="M9" s="7" t="s">
         <v>15</v>
@@ -1946,35 +1946,35 @@
       <c r="B27" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C27" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H27" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I27" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="J27" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K27" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="L27" s="7" t="s">
-        <v>15</v>
+      <c r="C27" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D27" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="E27" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="F27" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="G27" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="H27" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="I27" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="J27" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="K27" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="L27" s="7">
+        <v>0.5</v>
       </c>
       <c r="M27" s="7" t="s">
         <v>15</v>
@@ -2274,35 +2274,35 @@
       <c r="B35" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="C35" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G35" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H35" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I35" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="J35" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K35" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="L35" s="7" t="s">
-        <v>15</v>
+      <c r="C35" s="7">
+        <v>-0.5</v>
+      </c>
+      <c r="D35" s="7">
+        <v>-0.5</v>
+      </c>
+      <c r="E35" s="7">
+        <v>-0.5</v>
+      </c>
+      <c r="F35" s="7">
+        <v>-0.5</v>
+      </c>
+      <c r="G35" s="7">
+        <v>-0.5</v>
+      </c>
+      <c r="H35" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="I35" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="J35" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="K35" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="L35" s="7">
+        <v>0.5</v>
       </c>
       <c r="M35" s="7" t="s">
         <v>15</v>
@@ -2561,35 +2561,35 @@
       <c r="B42" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="C42" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F42" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G42" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H42" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I42" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="J42" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K42" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="L42" s="7" t="s">
-        <v>15</v>
+      <c r="C42" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D42" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="E42" s="7">
+        <v>-0.5</v>
+      </c>
+      <c r="F42" s="7">
+        <v>-0.5</v>
+      </c>
+      <c r="G42" s="7">
+        <v>-0.5</v>
+      </c>
+      <c r="H42" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="I42" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="J42" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="K42" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="L42" s="7">
+        <v>0.5</v>
       </c>
       <c r="M42" s="7" t="s">
         <v>15</v>
@@ -2734,26 +2734,26 @@
       <c r="E46" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F46" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G46" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H46" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I46" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="J46" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K46" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="L46" s="7" t="s">
-        <v>15</v>
+      <c r="F46" s="7">
+        <v>-0.5</v>
+      </c>
+      <c r="G46" s="7">
+        <v>-0.5</v>
+      </c>
+      <c r="H46" s="7">
+        <v>-0.5</v>
+      </c>
+      <c r="I46" s="7">
+        <v>0</v>
+      </c>
+      <c r="J46" s="7">
+        <v>-0.5</v>
+      </c>
+      <c r="K46" s="7">
+        <v>0</v>
+      </c>
+      <c r="L46" s="7">
+        <v>-0.5</v>
       </c>
       <c r="M46" s="7" t="s">
         <v>15</v>
@@ -2930,35 +2930,35 @@
       <c r="B51" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="C51" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E51" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F51" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G51" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H51" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I51" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="J51" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K51" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="L51" s="7" t="s">
-        <v>15</v>
+      <c r="C51" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D51" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="E51" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="F51" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="G51" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="H51" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="I51" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="J51" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="K51" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="L51" s="7">
+        <v>0.5</v>
       </c>
       <c r="M51" s="7" t="s">
         <v>15</v>
@@ -2972,34 +2972,34 @@
         <v>115</v>
       </c>
       <c r="C52" s="7">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="D52" s="7">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="E52" s="7">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="F52" s="7">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="G52" s="7">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="H52" s="7">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="I52" s="7">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="J52" s="7">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="K52" s="7">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="L52" s="7">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="M52" s="7">
         <v>0</v>
@@ -3013,34 +3013,34 @@
         <v>115</v>
       </c>
       <c r="C53" s="7">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D53" s="7">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E53" s="7">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="F53" s="7">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="G53" s="7">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="H53" s="7">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="I53" s="7">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="J53" s="7">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="K53" s="7">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="L53" s="7">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="M53" s="7">
         <v>0</v>
@@ -3054,13 +3054,13 @@
         <v>115</v>
       </c>
       <c r="C54" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D54" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E54" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F54" s="7">
         <v>0</v>
@@ -3095,34 +3095,34 @@
         <v>115</v>
       </c>
       <c r="C55" s="7">
-        <v>428</v>
+        <v>435</v>
       </c>
       <c r="D55" s="7">
-        <v>428</v>
+        <v>435</v>
       </c>
       <c r="E55" s="7">
-        <v>428</v>
+        <v>435</v>
       </c>
       <c r="F55" s="7">
-        <v>428</v>
+        <v>435</v>
       </c>
       <c r="G55" s="7">
-        <v>428</v>
+        <v>435</v>
       </c>
       <c r="H55" s="7">
-        <v>428</v>
+        <v>435</v>
       </c>
       <c r="I55" s="7">
-        <v>428</v>
+        <v>435</v>
       </c>
       <c r="J55" s="7">
-        <v>428</v>
+        <v>435</v>
       </c>
       <c r="K55" s="7">
-        <v>428</v>
+        <v>435</v>
       </c>
       <c r="L55" s="7">
-        <v>428</v>
+        <v>435</v>
       </c>
       <c r="M55" s="7">
         <v>0</v>
@@ -3136,34 +3136,34 @@
         <v>115</v>
       </c>
       <c r="C56" s="7">
+        <v>26</v>
+      </c>
+      <c r="D56" s="7">
+        <v>27</v>
+      </c>
+      <c r="E56" s="7">
+        <v>31.5</v>
+      </c>
+      <c r="F56" s="7">
         <v>24</v>
       </c>
-      <c r="D56" s="7">
-        <v>25</v>
-      </c>
-      <c r="E56" s="7">
-        <v>30</v>
-      </c>
-      <c r="F56" s="7">
-        <v>22</v>
-      </c>
       <c r="G56" s="7">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H56" s="7">
-        <v>34</v>
+        <v>36.5</v>
       </c>
       <c r="I56" s="7">
-        <v>43</v>
+        <v>45.5</v>
       </c>
       <c r="J56" s="7">
-        <v>42</v>
+        <v>44.5</v>
       </c>
       <c r="K56" s="7">
-        <v>41</v>
+        <v>43.5</v>
       </c>
       <c r="L56" s="7">
-        <v>33</v>
+        <v>35.5</v>
       </c>
       <c r="M56" s="7">
         <v>0</v>
@@ -3177,34 +3177,34 @@
         <v>115</v>
       </c>
       <c r="C57" s="7">
-        <v>-17</v>
+        <v>-17.5</v>
       </c>
       <c r="D57" s="7">
+        <v>-22.5</v>
+      </c>
+      <c r="E57" s="7">
+        <v>-18</v>
+      </c>
+      <c r="F57" s="7">
+        <v>-25.5</v>
+      </c>
+      <c r="G57" s="7">
+        <v>-33.5</v>
+      </c>
+      <c r="H57" s="7">
         <v>-22</v>
       </c>
-      <c r="E57" s="7">
-        <v>-17</v>
-      </c>
-      <c r="F57" s="7">
-        <v>-24</v>
-      </c>
-      <c r="G57" s="7">
-        <v>-32</v>
-      </c>
-      <c r="H57" s="7">
-        <v>-21</v>
-      </c>
       <c r="I57" s="7">
+        <v>-25.5</v>
+      </c>
+      <c r="J57" s="7">
         <v>-25</v>
       </c>
-      <c r="J57" s="7">
-        <v>-24</v>
-      </c>
       <c r="K57" s="7">
-        <v>-21</v>
+        <v>-21.5</v>
       </c>
       <c r="L57" s="7">
-        <v>-38</v>
+        <v>-39</v>
       </c>
       <c r="M57" s="7">
         <v>0</v>
@@ -3218,34 +3218,34 @@
         <v>115</v>
       </c>
       <c r="C58" s="7">
-        <v>7</v>
+        <v>8.5</v>
       </c>
       <c r="D58" s="7">
-        <v>3</v>
+        <v>4.5</v>
       </c>
       <c r="E58" s="7">
-        <v>13</v>
+        <v>13.5</v>
       </c>
       <c r="F58" s="7">
-        <v>-2</v>
+        <v>-1.5</v>
       </c>
       <c r="G58" s="7">
-        <v>-17</v>
+        <v>-16.5</v>
       </c>
       <c r="H58" s="7">
-        <v>13</v>
+        <v>14.5</v>
       </c>
       <c r="I58" s="7">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J58" s="7">
-        <v>18</v>
+        <v>19.5</v>
       </c>
       <c r="K58" s="7">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="L58" s="7">
-        <v>-5</v>
+        <v>-3.5</v>
       </c>
       <c r="M58" s="7">
         <v>0</v>
@@ -3264,7 +3264,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G42" sqref="G42"/>
+      <selection pane="bottomRight" activeCell="K66" sqref="K66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3390,45 +3390,45 @@
         <f>DATA!B3</f>
         <v xml:space="preserve"> Alaska</v>
       </c>
-      <c r="C3" s="10" t="str">
+      <c r="C3" s="10">
         <f>DATA!C3</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="D3" s="13" t="str">
+        <v>0</v>
+      </c>
+      <c r="D3" s="13">
         <f>DATA!D3</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="E3" s="10" t="str">
+        <v>0</v>
+      </c>
+      <c r="E3" s="10">
         <f>DATA!E3</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="F3" s="10" t="str">
+        <v>0</v>
+      </c>
+      <c r="F3" s="10">
         <f>DATA!F3</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="G3" s="10" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="G3" s="10">
         <f>DATA!G3</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="H3" s="10" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="H3" s="10">
         <f>DATA!H3</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="I3" s="13" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="I3" s="13">
         <f>DATA!I3</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="J3" s="10" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="J3" s="10">
         <f>DATA!J3</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="K3" s="10" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="K3" s="10">
         <f>DATA!K3</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="L3" s="10" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="L3" s="10">
         <f>DATA!L3</f>
-        <v xml:space="preserve"> None</v>
+        <v>0.5</v>
       </c>
       <c r="M3" s="10" t="str">
         <f>DATA!M3</f>
@@ -3720,45 +3720,45 @@
         <f>DATA!B9</f>
         <v xml:space="preserve"> Delaware</v>
       </c>
-      <c r="C9" s="10" t="str">
+      <c r="C9" s="10">
         <f>DATA!C9</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="D9" s="13" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="D9" s="13">
         <f>DATA!D9</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="E9" s="10" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="E9" s="10">
         <f>DATA!E9</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="F9" s="10" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="F9" s="10">
         <f>DATA!F9</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="G9" s="10" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="G9" s="10">
         <f>DATA!G9</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="H9" s="10" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="H9" s="10">
         <f>DATA!H9</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="I9" s="13" t="str">
+        <v>-0.5</v>
+      </c>
+      <c r="I9" s="13">
         <f>DATA!I9</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="J9" s="10" t="str">
+        <v>-0.5</v>
+      </c>
+      <c r="J9" s="10">
         <f>DATA!J9</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="K9" s="10" t="str">
+        <v>-0.5</v>
+      </c>
+      <c r="K9" s="10">
         <f>DATA!K9</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="L9" s="10" t="str">
+        <v>-0.5</v>
+      </c>
+      <c r="L9" s="10">
         <f>DATA!L9</f>
-        <v xml:space="preserve"> None</v>
+        <v>-0.5</v>
       </c>
       <c r="M9" s="10" t="str">
         <f>DATA!M9</f>
@@ -4710,45 +4710,45 @@
         <f>DATA!B27</f>
         <v xml:space="preserve"> Montana</v>
       </c>
-      <c r="C27" s="10" t="str">
+      <c r="C27" s="10">
         <f>DATA!C27</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="D27" s="13" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="D27" s="13">
         <f>DATA!D27</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="E27" s="10" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="E27" s="10">
         <f>DATA!E27</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="F27" s="10" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="F27" s="10">
         <f>DATA!F27</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="G27" s="10" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="G27" s="10">
         <f>DATA!G27</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="H27" s="10" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="H27" s="10">
         <f>DATA!H27</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="I27" s="13" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="I27" s="13">
         <f>DATA!I27</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="J27" s="10" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="J27" s="10">
         <f>DATA!J27</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="K27" s="10" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="K27" s="10">
         <f>DATA!K27</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="L27" s="10" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="L27" s="10">
         <f>DATA!L27</f>
-        <v xml:space="preserve"> None</v>
+        <v>0.5</v>
       </c>
       <c r="M27" s="10" t="str">
         <f>DATA!M27</f>
@@ -5150,45 +5150,45 @@
         <f>DATA!B35</f>
         <v xml:space="preserve"> North Dakota</v>
       </c>
-      <c r="C35" s="10" t="str">
+      <c r="C35" s="10">
         <f>DATA!C35</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="D35" s="13" t="str">
+        <v>-0.5</v>
+      </c>
+      <c r="D35" s="13">
         <f>DATA!D35</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="E35" s="10" t="str">
+        <v>-0.5</v>
+      </c>
+      <c r="E35" s="10">
         <f>DATA!E35</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="F35" s="10" t="str">
+        <v>-0.5</v>
+      </c>
+      <c r="F35" s="10">
         <f>DATA!F35</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="G35" s="10" t="str">
+        <v>-0.5</v>
+      </c>
+      <c r="G35" s="10">
         <f>DATA!G35</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="H35" s="10" t="str">
+        <v>-0.5</v>
+      </c>
+      <c r="H35" s="10">
         <f>DATA!H35</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="I35" s="13" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="I35" s="13">
         <f>DATA!I35</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="J35" s="10" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="J35" s="10">
         <f>DATA!J35</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="K35" s="10" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="K35" s="10">
         <f>DATA!K35</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="L35" s="10" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="L35" s="10">
         <f>DATA!L35</f>
-        <v xml:space="preserve"> None</v>
+        <v>0.5</v>
       </c>
       <c r="M35" s="10" t="str">
         <f>DATA!M35</f>
@@ -5535,45 +5535,45 @@
         <f>DATA!B42</f>
         <v xml:space="preserve"> South Dakota</v>
       </c>
-      <c r="C42" s="10" t="str">
+      <c r="C42" s="10">
         <f>DATA!C42</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="D42" s="13" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="D42" s="13">
         <f>DATA!D42</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="E42" s="10" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="E42" s="10">
         <f>DATA!E42</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="F42" s="10" t="str">
+        <v>-0.5</v>
+      </c>
+      <c r="F42" s="10">
         <f>DATA!F42</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="G42" s="10" t="str">
+        <v>-0.5</v>
+      </c>
+      <c r="G42" s="10">
         <f>DATA!G42</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="H42" s="10" t="str">
+        <v>-0.5</v>
+      </c>
+      <c r="H42" s="10">
         <f>DATA!H42</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="I42" s="13" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="I42" s="13">
         <f>DATA!I42</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="J42" s="10" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="J42" s="10">
         <f>DATA!J42</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="K42" s="10" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="K42" s="10">
         <f>DATA!K42</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="L42" s="10" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="L42" s="10">
         <f>DATA!L42</f>
-        <v xml:space="preserve"> None</v>
+        <v>0.5</v>
       </c>
       <c r="M42" s="10" t="str">
         <f>DATA!M42</f>
@@ -5767,33 +5767,33 @@
         <f>DATA!E46</f>
         <v xml:space="preserve"> None</v>
       </c>
-      <c r="F46" s="10" t="str">
+      <c r="F46" s="10">
         <f>DATA!F46</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="G46" s="10" t="str">
+        <v>-0.5</v>
+      </c>
+      <c r="G46" s="10">
         <f>DATA!G46</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="H46" s="10" t="str">
+        <v>-0.5</v>
+      </c>
+      <c r="H46" s="10">
         <f>DATA!H46</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="I46" s="13" t="str">
+        <v>-0.5</v>
+      </c>
+      <c r="I46" s="13">
         <f>DATA!I46</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="J46" s="10" t="str">
+        <v>0</v>
+      </c>
+      <c r="J46" s="10">
         <f>DATA!J46</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="K46" s="10" t="str">
+        <v>-0.5</v>
+      </c>
+      <c r="K46" s="10">
         <f>DATA!K46</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="L46" s="10" t="str">
+        <v>0</v>
+      </c>
+      <c r="L46" s="10">
         <f>DATA!L46</f>
-        <v xml:space="preserve"> None</v>
+        <v>-0.5</v>
       </c>
       <c r="M46" s="10" t="str">
         <f>DATA!M46</f>
@@ -6030,45 +6030,45 @@
         <f>DATA!B51</f>
         <v xml:space="preserve"> Wyoming</v>
       </c>
-      <c r="C51" s="11" t="str">
+      <c r="C51" s="11">
         <f>DATA!C51</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="D51" s="14" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="D51" s="14">
         <f>DATA!D51</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="E51" s="11" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="E51" s="11">
         <f>DATA!E51</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="F51" s="11" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="F51" s="11">
         <f>DATA!F51</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="G51" s="11" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="G51" s="11">
         <f>DATA!G51</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="H51" s="11" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="H51" s="11">
         <f>DATA!H51</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="I51" s="14" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="I51" s="14">
         <f>DATA!I51</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="J51" s="11" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="J51" s="11">
         <f>DATA!J51</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="K51" s="11" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="K51" s="11">
         <f>DATA!K51</f>
-        <v xml:space="preserve"> None</v>
-      </c>
-      <c r="L51" s="11" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="L51" s="11">
         <f>DATA!L51</f>
-        <v xml:space="preserve"> None</v>
+        <v>0.5</v>
       </c>
       <c r="M51" s="11" t="str">
         <f>DATA!M51</f>
@@ -6103,43 +6103,43 @@
       </c>
       <c r="C53" s="10">
         <f>DATA!C52</f>
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="D53" s="13">
         <f>DATA!D52</f>
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="E53" s="10">
         <f>DATA!E52</f>
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="F53" s="10">
         <f>DATA!F52</f>
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="G53" s="10">
         <f>DATA!G52</f>
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="H53" s="10">
         <f>DATA!H52</f>
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="I53" s="13">
         <f>DATA!I52</f>
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="J53" s="10">
         <f>DATA!J52</f>
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="K53" s="10">
         <f>DATA!K52</f>
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="L53" s="10">
         <f>DATA!L52</f>
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="M53" s="10">
         <f>DATA!M52</f>
@@ -6158,43 +6158,43 @@
       </c>
       <c r="C54" s="10">
         <f>DATA!C53</f>
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D54" s="13">
         <f>DATA!D53</f>
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E54" s="10">
         <f>DATA!E53</f>
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="F54" s="10">
         <f>DATA!F53</f>
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="G54" s="10">
         <f>DATA!G53</f>
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="H54" s="10">
         <f>DATA!H53</f>
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="I54" s="13">
         <f>DATA!I53</f>
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="J54" s="10">
         <f>DATA!J53</f>
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="K54" s="10">
         <f>DATA!K53</f>
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="L54" s="10">
         <f>DATA!L53</f>
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="M54" s="10">
         <f>DATA!M53</f>
@@ -6213,15 +6213,15 @@
       </c>
       <c r="C55" s="11">
         <f>DATA!C54</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D55" s="14">
         <f>DATA!D54</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E55" s="11">
         <f>DATA!E54</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F55" s="11">
         <f>DATA!F54</f>
@@ -6268,43 +6268,43 @@
       </c>
       <c r="C56" s="10">
         <f>DATA!C55</f>
-        <v>428</v>
+        <v>435</v>
       </c>
       <c r="D56" s="13">
         <f>DATA!D55</f>
-        <v>428</v>
+        <v>435</v>
       </c>
       <c r="E56" s="10">
         <f>DATA!E55</f>
-        <v>428</v>
+        <v>435</v>
       </c>
       <c r="F56" s="10">
         <f>DATA!F55</f>
-        <v>428</v>
+        <v>435</v>
       </c>
       <c r="G56" s="10">
         <f>DATA!G55</f>
-        <v>428</v>
+        <v>435</v>
       </c>
       <c r="H56" s="10">
         <f>DATA!H55</f>
-        <v>428</v>
+        <v>435</v>
       </c>
       <c r="I56" s="13">
         <f>DATA!I55</f>
-        <v>428</v>
+        <v>435</v>
       </c>
       <c r="J56" s="10">
         <f>DATA!J55</f>
-        <v>428</v>
+        <v>435</v>
       </c>
       <c r="K56" s="10">
         <f>DATA!K55</f>
-        <v>428</v>
+        <v>435</v>
       </c>
       <c r="L56" s="10">
         <f>DATA!L55</f>
-        <v>428</v>
+        <v>435</v>
       </c>
       <c r="M56" s="10">
         <f>DATA!M55</f>
@@ -6339,43 +6339,43 @@
       </c>
       <c r="C58" s="10">
         <f>DATA!C56</f>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D58" s="13">
         <f>DATA!D56</f>
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E58" s="10">
         <f>DATA!E56</f>
-        <v>30</v>
+        <v>31.5</v>
       </c>
       <c r="F58" s="10">
         <f>DATA!F56</f>
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G58" s="10">
         <f>DATA!G56</f>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H58" s="10">
         <f>DATA!H56</f>
-        <v>34</v>
+        <v>36.5</v>
       </c>
       <c r="I58" s="13">
         <f>DATA!I56</f>
-        <v>43</v>
+        <v>45.5</v>
       </c>
       <c r="J58" s="10">
         <f>DATA!J56</f>
-        <v>42</v>
+        <v>44.5</v>
       </c>
       <c r="K58" s="10">
         <f>DATA!K56</f>
-        <v>41</v>
+        <v>43.5</v>
       </c>
       <c r="L58" s="10">
         <f>DATA!L56</f>
-        <v>33</v>
+        <v>35.5</v>
       </c>
       <c r="M58" s="10">
         <f>DATA!M56</f>
@@ -6394,43 +6394,43 @@
       </c>
       <c r="C59" s="11">
         <f>DATA!C57</f>
-        <v>-17</v>
+        <v>-17.5</v>
       </c>
       <c r="D59" s="14">
         <f>DATA!D57</f>
-        <v>-22</v>
+        <v>-22.5</v>
       </c>
       <c r="E59" s="11">
         <f>DATA!E57</f>
-        <v>-17</v>
+        <v>-18</v>
       </c>
       <c r="F59" s="11">
         <f>DATA!F57</f>
-        <v>-24</v>
+        <v>-25.5</v>
       </c>
       <c r="G59" s="11">
         <f>DATA!G57</f>
-        <v>-32</v>
+        <v>-33.5</v>
       </c>
       <c r="H59" s="11">
         <f>DATA!H57</f>
-        <v>-21</v>
+        <v>-22</v>
       </c>
       <c r="I59" s="14">
         <f>DATA!I57</f>
-        <v>-25</v>
+        <v>-25.5</v>
       </c>
       <c r="J59" s="11">
         <f>DATA!J57</f>
-        <v>-24</v>
+        <v>-25</v>
       </c>
       <c r="K59" s="11">
         <f>DATA!K57</f>
-        <v>-21</v>
+        <v>-21.5</v>
       </c>
       <c r="L59" s="11">
         <f>DATA!L57</f>
-        <v>-38</v>
+        <v>-39</v>
       </c>
       <c r="M59" s="11">
         <f>DATA!M57</f>
@@ -6449,43 +6449,43 @@
       </c>
       <c r="C60" s="10">
         <f>DATA!C58</f>
-        <v>7</v>
+        <v>8.5</v>
       </c>
       <c r="D60" s="13">
         <f>DATA!D58</f>
-        <v>3</v>
+        <v>4.5</v>
       </c>
       <c r="E60" s="10">
         <f>DATA!E58</f>
-        <v>13</v>
+        <v>13.5</v>
       </c>
       <c r="F60" s="10">
         <f>DATA!F58</f>
-        <v>-2</v>
+        <v>-1.5</v>
       </c>
       <c r="G60" s="10">
         <f>DATA!G58</f>
-        <v>-17</v>
+        <v>-16.5</v>
       </c>
       <c r="H60" s="10">
         <f>DATA!H58</f>
-        <v>13</v>
+        <v>14.5</v>
       </c>
       <c r="I60" s="13">
         <f>DATA!I58</f>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J60" s="10">
         <f>DATA!J58</f>
-        <v>18</v>
+        <v>19.5</v>
       </c>
       <c r="K60" s="10">
         <f>DATA!K58</f>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="L60" s="10">
         <f>DATA!L58</f>
-        <v>-5</v>
+        <v>-3.5</v>
       </c>
       <c r="M60" s="10">
         <f>DATA!M58</f>

</xml_diff>